<commit_message>
running baseline again for correct results
</commit_message>
<xml_diff>
--- a/QALD9-Plus-testing/baseline-model/baseline_dbpedia_wikidata/baseline_comparison_results_llama.xlsx
+++ b/QALD9-Plus-testing/baseline-model/baseline_dbpedia_wikidata/baseline_comparison_results_llama.xlsx
@@ -1,96 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meine Ablage\Master Thesis\SPARQL-Query-Translation-QALD9\QALD9-Plus-testing\baseline-model\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F02A3452-F127-4BEC-98BF-BAF7F513F4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>question</t>
-  </si>
-  <si>
-    <t>expected_answers</t>
-  </si>
-  <si>
-    <t>lama_answers</t>
-  </si>
-  <si>
-    <t>is_correct</t>
-  </si>
-  <si>
-    <t>Which city has the least inhabitants?</t>
-  </si>
-  <si>
-    <t>['http://www.wikidata.org/entity/Q2590944']</t>
-  </si>
-  <si>
-    <t>['http://www.wikidata.org/entity/Q1000143', 'http://www.wikidata.org/entity/Q1000333', 'http://www.wikidata.org/entity/Q1000341', 'http://www.wikidata.org/entity/Q1000346', 'http://www.wikidata.org/entity/Q1000373', 'http://www.wikidata.org/entity/Q1000438', 'http://www.wikidata.org/entity/Q1000495', 'http://www.wikidata.org/entity/Q10006', 'http://www.wikidata.org/entity/Q1000609', 'http://www.wikidata.org/entity/Q1000839', 'http://www.wikidata.org/entity/Q1000844', 'http://www.wikidata.org/entity/Q1000883', 'http://www.wikidata.org/entity/Q1000887', 'http://www.wikidata.org/entity/Q1000938', 'http://www.wikidata.org/entity/Q1001200', 'http://www.wikidata.org/entity/Q1001307', 'http://www.wikidata.org/entity/Q1001322', 'http://www.wikidata.org/entity/Q10014', 'http://www.wikidata.org/entity/Q1001440', 'http://www.wikidata.org/entity/Q1001496', 'http://www.wikidata.org/entity/Q1001517', 'http://www.wikidata.org/entity/Q1001522', 'http://www.wikidata.org/entity/Q1001571', 'http://www.wikidata.org/entity/Q1001758', 'http://www.wikidata.org/entity/Q1001817', 'http://www.wikidata.org/entity/Q100188', 'http://www.wikidata.org/entity/Q1001887', 'http://www.wikidata.org/entity/Q1001897', 'http://www.wikidata.org/entity/Q1001914', 'http://www.wikidata.org/entity/Q1001941', 'http://www.wikidata.org/entity/Q1001959', 'http://www.wikidata.org/entity/Q1001989', 'http://www.wikidata.org/entity/Q1001995', 'http://www.wikidata.org/entity/Q1002035', 'http://www.wikidata.org/entity/Q1002052', 'http://www.wikidata.org/entity/Q1002076', 'http://www.wikidata.org/entity/Q1002084', 'http://www.wikidata.org/entity/Q1002105', 'http://www.wikidata.org/entity/Q1002144', 'http://www.wikidata.org/entity/Q1002286', 'http://www.wikidata.org/entity/Q100234030', 'http://www.wikidata.org/entity/Q1002533', 'http://www.wikidata.org/entity/Q1002557', 'http://www.wikidata.org/entity/Q1002560', 'http://www.wikidata.org/entity/Q1002580', 'http://www.wikidata.org/entity/Q1002638', 'http://www.wikidata.org/entity/Q1002658', 'http://www.wikidata.org/entity/Q1002670', 'http://www.wikidata.org/entity/Q1002685', 'http://www.wikidata.org/entity/Q1002696', 'http://www.wikidata.org/entity/Q1002776', 'http://www.wikidata.org/entity/Q1002807', 'http://www.wikidata.org/entity/Q1002823', 'http://www.wikidata.org/entity/Q1002841', 'http://www.wikidata.org/entity/Q1002900', 'http://www.wikidata.org/entity/Q1002944', 'http://www.wikidata.org/entity/Q1003016', 'http://www.wikidata.org/entity/Q1003112', 'http://www.wikidata.org/entity/Q1003264', 'http://www.wikidata.org/entity/Q1003267', 'http://www.wikidata.org/entity/Q1003272', 'http://www.wikidata.org/entity/Q1003276', 'http://www.wikidata.org/entity/Q1003279', 'http://www.wikidata.org/entity/Q1003283', 'http://www.wikidata.org/entity/Q1003302', 'http://www.wikidata.org/entity/Q1003318', 'http://www.wikidata.org/entity/Q1003328', 'http://www.wikidata.org/entity/Q1003511', 'http://www.wikidata.org/entity/Q1003903', 'http://www.wikidata.org/entity/Q1004048', 'http://www.wikidata.org/entity/Q1004283', 'http://www.wikidata.org/entity/Q1004290', 'http://www.wikidata.org/entity/Q1004295', 'http://www.wikidata.org/entity/Q1004298', 'http://www.wikidata.org/entity/Q1004302', 'http://www.wikidata.org/entity/Q1004312', 'http://www.wikidata.org/entity/Q1004320', 'http://www.wikidata.org/entity/Q1004328', 'http://www.wikidata.org/entity/Q10045', 'http://www.wikidata.org/entity/Q1004686', 'http://www.wikidata.org/entity/Q1004716', 'http://www.wikidata.org/entity/Q1004822', 'http://www.wikidata.org/entity/Q10052', 'http://www.wikidata.org/entity/Q1005350', 'http://www.wikidata.org/entity/Q1005356', 'http://www.wikidata.org/entity/Q1005359', 'http://www.wikidata.org/entity/Q1005384', 'http://www.wikidata.org/entity/Q1005394', 'http://www.wikidata.org/entity/Q1005403', 'http://www.wikidata.org/entity/Q1005409', 'http://www.wikidata.org/entity/Q1005414', 'http://www.wikidata.org/entity/Q1005419', 'http://www.wikidata.org/entity/Q1005428', 'http://www.wikidata.org/entity/Q1005435', 'http://www.wikidata.org/entity/Q1005442', 'http://www.wikidata.org/entity/Q10054424', 'http://www.wikidata.org/entity/Q1005453', 'http://www.wikidata.org/entity/Q1005464', 'http://www.wikidata.org/entity/Q1005472', 'http://www.wikidata.org/entity/Q1005483', 'http://www.wikidata.org/entity/Q1005492', 'http://www.wikidata.org/entity/Q1005503', 'http://www.wikidata.org/entity/Q1005511', 'http://www.wikidata.org/entity/Q1005538', 'http://www.wikidata.org/entity/Q1005584', 'http://www.wikidata.org/entity/Q1005725', 'http://www.wikidata.org/entity/Q1005770', 'http://www.wikidata.org/entity/Q1005786', 'http://www.wikidata.org/entity/Q1005827', 'http://www.wikidata.org/entity/Q1005837', 'http://www.wikidata.org/entity/Q1005855', 'http://www.wikidata.org/entity/Q1005885', 'http://www.wikidata.org/entity/Q1005905', 'http://www.wikidata.org/entity/Q1005972', 'http://www.wikidata.org/entity/Q1006081', 'http://www.wikidata.org/entity/Q1006116', 'http://www.wikidata.org/entity/Q1006137', 'http://www.wikidata.org/entity/Q1006155', 'http://www.wikidata.org/entity/Q1006165', 'http://www.wikidata.org/entity/Q1006240', 'http://www.wikidata.org/entity/Q1006277', 'http://www.wikidata.org/entity/Q1006296', 'http://www.wikidata.org/entity/Q1006303', 'http://www.wikidata.org/entity/Q1006321', 'http://www.wikidata.org/entity/Q1006343', 'http://www.wikidata.org/entity/Q1006350', 'http://www.wikidata.org/entity/Q1006355', 'http://www.wikidata.org/entity/Q1006363', 'http://www.wikidata.org/entity/Q1006764', 'http://www.wikidata.org/entity/Q1006772', 'http://www.wikidata.org/entity/Q1006788', 'http://www.wikidata.org/entity/Q1006813', 'http://www.wikidata.org/entity/Q1007232', 'http://www.wikidata.org/entity/Q1007275', 'http://www.wikidata.org/entity/Q1007342', 'http://www.wikidata.org/entity/Q1007355', 'http://www.wikidata.org/entity/Q1007407', 'http://www.wikidata.org/entity/Q1007479', 'http://www.wikidata.org/entity/Q1007576', 'http://www.wikidata.org/entity/Q1007634', 'http://www.wikidata.org/entity/Q1007647', 'http://www.wikidata.org/entity/Q1007702', 'http://www.wikidata.org/entity/Q1007719', 'http://www.wikidata.org/entity/Q1008008', 'http://www.wikidata.org/entity/Q1008152', 'http://www.wikidata.org/entity/Q1008368', 'http://www.wikidata.org/entity/Q1008390', 'http://www.wikidata.org/entity/Q1008456', 'http://www.wikidata.org/entity/Q10086', 'http://www.wikidata.org/entity/Q1008761', 'http://www.wikidata.org/entity/Q1008853', 'http://www.wikidata.org/entity/Q1008963', 'http://www.wikidata.org/entity/Q1009161', 'http://www.wikidata.org/entity/Q1009179', 'http://www.wikidata.org/entity/Q1009199', 'http://www.wikidata.org/entity/Q1009253', 'http://www.wikidata.org/entity/Q1009276', 'http://www.wikidata.org/entity/Q1009308', 'http://www.wikidata.org/entity/Q1009336', 'http://www.wikidata.org/entity/Q1009509', 'http://www.wikidata.org/entity/Q1009549', 'http://www.wikidata.org/entity/Q1009864', 'http://www.wikidata.org/entity/Q1010', 'http://www.wikidata.org/entity/Q101002825', 'http://www.wikidata.org/entity/Q1010153', 'http://www.wikidata.org/entity/Q1010278', 'http://www.wikidata.org/entity/Q1010287', 'http://www.wikidata.org/entity/Q1010367', 'http://www.wikidata.org/entity/Q1010806', 'http://www.wikidata.org/entity/Q1010816', 'http://www.wikidata.org/entity/Q1010823', 'http://www.wikidata.org/entity/Q1010954', 'http://www.wikidata.org/entity/Q1010960', 'http://www.wikidata.org/entity/Q1010979', 'http://www.wikidata.org/entity/Q1010985', 'http://www.wikidata.org/entity/Q1011011', 'http://www.wikidata.org/entity/Q1011016', 'http://www.wikidata.org/entity/Q1011047', 'http://www.wikidata.org/entity/Q101145616', 'http://www.wikidata.org/entity/Q1011488', 'http://www.wikidata.org/entity/Q1011553', 'http://www.wikidata.org/entity/Q1011669', 'http://www.wikidata.org/entity/Q1011819', 'http://www.wikidata.org/entity/Q1011863', 'http://www.wikidata.org/entity/Q1011873', 'http://www.wikidata.org/entity/Q1011882', 'http://www.wikidata.org/entity/Q1011890', 'http://www.wikidata.org/entity/Q1011972', 'http://www.wikidata.org/entity/Q1012', 'http://www.wikidata.org/entity/Q101254', 'http://www.wikidata.org/entity/Q1012706', 'http://www.wikidata.org/entity/Q1012828', 'http://www.wikidata.org/entity/Q1012831', 'http://www.wikidata.org/entity/Q101283288', 'http://www.wikidata.org/entity/Q1012862', 'http://www.wikidata.org/entity/Q1012868', 'http://www.wikidata.org/entity/Q1012881', 'http://www.wikidata.org/entity/Q1012887', 'http://www.wikidata.org/entity/Q1012924', 'http://www.wikidata.org/entity/Q1013119', 'http://www.wikidata.org/entity/Q1013379', 'http://www.wikidata.org/entity/Q1013424', 'http://www.wikidata.org/entity/Q1013428', 'http://www.wikidata.org/entity/Q1013454', 'http://www.wikidata.org/entity/Q1013526', 'http://www.wikidata.org/entity/Q1013831', 'http://www.wikidata.org/entity/Q1013946', 'http://www.wikidata.org/entity/Q1013965', 'http://www.wikidata.org/entity/Q1014010', 'http://www.wikidata.org/entity/Q101418', 'http://www.wikidata.org/entity/Q1014231', 'http://www.wikidata.org/entity/Q1014235', 'http://www.wikidata.org/entity/Q1014248', 'http://www.wikidata.org/entity/Q1014285', 'http://www.wikidata.org/entity/Q1014306', 'http://www.wikidata.org/entity/Q1014315', 'http://www.wikidata.org/entity/Q1014367', 'http://www.wikidata.org/entity/Q1014375', 'http://www.wikidata.org/entity/Q1014380', 'http://www.wikidata.org/entity/Q1014390', 'http://www.wikidata.org/entity/Q1014423', 'http://www.wikidata.org/entity/Q1014430', 'http://www.wikidata.org/entity/Q1014433', 'http://www.wikidata.org/entity/Q1014456', 'http://www.wikidata.org/entity/Q1014461', 'http://www.wikidata.org/entity/Q1014468', 'http://www.wikidata.org/entity/Q1014474', 'http://www.wikidata.org/entity/Q1014481', 'http://www.wikidata.org/entity/Q1014493', 'http://www.wikidata.org/entity/Q1014504', 'http://www.wikidata.org/entity/Q1014511', 'http://www.wikidata.org/entity/Q1014530', 'http://www.wikidata.org/entity/Q1014543', 'http://www.wikidata.org/entity/Q1014554', 'http://www.wikidata.org/entity/Q1014561', 'http://www.wikidata.org/entity/Q1014564', 'http://www.wikidata.org/entity/Q1014661', 'http://www.wikidata.org/entity/Q1015', 'http://www.wikidata.org/entity/Q1015036', 'http://www.wikidata.org/entity/Q1015069', 'http://www.wikidata.org/entity/Q1015146', 'http://www.wikidata.org/entity/Q1015152', 'http://www.wikidata.org/entity/Q1015160', 'http://www.wikidata.org/entity/Q1015165', 'http://www.wikidata.org/entity/Q1015172', 'http://www.wikidata.org/entity/Q101530', 'http://www.wikidata.org/entity/Q1015472', 'http://www.wikidata.org/entity/Q1015546', 'http://www.wikidata.org/entity/Q1015618', 'http://www.wikidata.org/entity/Q1015639', 'http://www.wikidata.org/entity/Q1015672', 'http://www.wikidata.org/entity/Q1015681', 'http://www.wikidata.org/entity/Q1015690', 'http://www.wikidata.org/entity/Q1015699', 'http://www.wikidata.org/entity/Q1015727', 'http://www.wikidata.org/entity/Q1015752', 'http://www.wikidata.org/entity/Q1015773', 'http://www.wikidata.org/entity/Q1015796', 'http://www.wikidata.org/entity/Q1015891', 'http://www.wikidata.org/entity/Q1016047', 'http://www.wikidata.org/entity/Q101625', 'http://www.wikidata.org/entity/Q1016289', 'http://www.wikidata.org/entity/Q1016827', 'http://www.wikidata.org/entity/Q1016873', 'http://www.wikidata.org/entity/Q1016881', 'http://www.wikidata.org/entity/Q101704', 'http://www.wikidata.org/entity/Q1017098', 'http://www.wikidata.org/entity/Q1017120', 'http://www.wikidata.org/entity/Q1017160', 'http://www.wikidata.org/entity/Q1017167', 'http://www.wikidata.org/entity/Q1017183', 'http://www.wikidata.org/entity/Q1017205', 'http://www.wikidata.org/entity/Q1017208', 'http://www.wikidata.org/entity/Q1017210', 'http://www.wikidata.org/entity/Q1017314', 'http://www.wikidata.org/entity/Q1017331', 'http://www.wikidata.org/entity/Q1017358', 'http://www.wikidata.org/entity/Q1017362', 'http://www.wikidata.org/entity/Q1017367', 'http://www.wikidata.org/entity/Q1017369', 'http://www.wikidata.org/entity/Q1017376', 'http://www.wikidata.org/entity/Q1017387', 'http://www.wikidata.org/entity/Q1017430', 'http://www.wikidata.org/entity/Q1017554', 'http://www.wikidata.org/entity/Q1017556', 'http://www.wikidata.org/entity/Q1017594', 'http://www.wikidata.org/entity/Q1017624', 'http://www.wikidata.org/entity/Q1017630', 'http://www.wikidata.org/entity/Q1017637', 'http://www.wikidata.org/entity/Q1017644', 'http://www.wikidata.org/entity/Q1017651', 'http://www.wikidata.org/entity/Q1017662', 'http://www.wikidata.org/entity/Q1017673', 'http://www.wikidata.org/entity/Q1017678', 'http://www.wikidata.org/entity/Q1017683', 'http://www.wikidata.org/entity/Q1017691', 'http://www.wikidata.org/entity/Q1017696', 'http://www.wikidata.org/entity/Q1017710', 'http://www.wikidata.org/entity/Q1017735', 'http://www.wikidata.org/entity/Q1017801', 'http://www.wikidata.org/entity/Q1017895', 'http://www.wikidata.org/entity/Q1017971', 'http://www.wikidata.org/entity/Q1018016', 'http://www.wikidata.org/entity/Q1018092', 'http://www.wikidata.org/entity/Q1018116', 'http://www.wikidata.org/entity/Q1018160', 'http://www.wikidata.org/entity/Q1018163', 'http://www.wikidata.org/entity/Q1018167', 'http://www.wikidata.org/entity/Q1018173', 'http://www.wikidata.org/entity/Q1018201', 'http://www.wikidata.org/entity/Q1018215', 'http://www.wikidata.org/entity/Q1018239', 'http://www.wikidata.org/entity/Q1018271', 'http://www.wikidata.org/entity/Q1018369', 'http://www.wikidata.org/entity/Q1018501', 'http://www.wikidata.org/entity/Q1018524', 'http://www.wikidata.org/entity/Q1018574', 'http://www.wikidata.org/entity/Q1018584', 'http://www.wikidata.org/entity/Q1018592', 'http://www.wikidata.org/entity/Q1018693', 'http://www.wikidata.org/entity/Q1018701', 'http://www.wikidata.org/entity/Q1018781', 'http://www.wikidata.org/entity/Q1018868', 'http://www.wikidata.org/entity/Q1018872', 'http://www.wikidata.org/entity/Q1018877', 'http://www.wikidata.org/entity/Q1019060', 'http://www.wikidata.org/entity/Q1019120', 'http://www.wikidata.org/entity/Q1019152', 'http://www.wikidata.org/entity/Q1019287', 'http://www.wikidata.org/entity/Q1019356', 'http://www.wikidata.org/entity/Q1019377', 'http://www.wikidata.org/entity/Q1019402', 'http://www.wikidata.org/entity/Q1019405', 'http://www.wikidata.org/entity/Q1019424', 'http://www.wikidata.org/entity/Q1019429', 'http://www.wikidata.org/entity/Q1019431', 'http://www.wikidata.org/entity/Q1019443', 'http://www.wikidata.org/entity/Q1019448', 'http://www.wikidata.org/entity/Q1019452', 'http://www.wikidata.org/entity/Q1019466', 'http://www.wikidata.org/entity/Q1019470', 'http://www.wikidata.org/entity/Q1019496', 'http://www.wikidata.org/entity/Q1019505', 'http://www.wikidata.org/entity/Q1019534', 'http://www.wikidata.org/entity/Q1019991', 'http://www.wikidata.org/entity/Q1020010', 'http://www.wikidata.org/entity/Q1020110', 'http://www.wikidata.org/entity/Q1020261', 'http://www.wikidata.org/entity/Q1020263', 'http://www.wikidata.org/entity/Q1020273', 'http://www.wikidata.org/entity/Q1020276', 'http://www.wikidata.org/entity/Q1020277', 'http://www.wikidata.org/entity/Q1020279', 'http://www.wikidata.org/entity/Q1020288', 'http://www.wikidata.org/entity/Q1020292', 'http://www.wikidata.org/entity/Q1020297', 'http://www.wikidata.org/entity/Q1020309', 'http://www.wikidata.org/entity/Q1020314', 'http://www.wikidata.org/entity/Q1020320', 'http://www.wikidata.org/entity/Q1020338', 'http://www.wikidata.org/entity/Q1020384', 'http://www.wikidata.org/entity/Q1020396', 'http://www.wikidata.org/entity/Q1020477', 'http://www.wikidata.org/entity/Q1020481', 'http://www.wikidata.org/entity/Q1020484', 'http://www.wikidata.org/entity/Q1020490', 'http://www.wikidata.org/entity/Q1020535', 'http://www.wikidata.org/entity/Q1020627', 'http://www.wikidata.org/entity/Q1020649', 'http://www.wikidata.org/entity/Q1020718', 'http://www.wikidata.org/entity/Q1020762', 'http://www.wikidata.org/entity/Q1020776', 'http://www.wikidata.org/entity/Q1020785', 'http://www.wikidata.org/entity/Q1020794', 'http://www.wikidata.org/entity/Q1020853', 'http://www.wikidata.org/entity/Q1020969', 'http://www.wikidata.org/entity/Q1020997', 'http://www.wikidata.org/entity/Q1021', 'http://www.wikidata.org/entity/Q1021013', 'http://www.wikidata.org/entity/Q1021223', 'http://www.wikidata.org/entity/Q1021263', 'http://www.wikidata.org/entity/Q1021272', 'http://www.wikidata.org/entity/Q1021277', 'http://www.wikidata.org/entity/Q1021282', 'http://www.wikidata.org/entity/Q1021286', 'http://www.wikidata.org/entity/Q1021294', 'http://www.wikidata.org/entity/Q1021592', 'http://www.wikidata.org/entity/Q1021638', 'http://www.wikidata.org/entity/Q1021800', 'http://www.wikidata.org/entity/Q102180841', 'http://www.wikidata.org/entity/Q1021903', 'http://www.wikidata.org/entity/Q1022131', 'http://www.wikidata.org/entity/Q1022152', 'http://www.wikidata.org/entity/Q1022170', 'http://www.wikidata.org/entity/Q1022481', 'http://www.wikidata.org/entity/Q1022488', 'http://www.wikidata.org/entity/Q1022523', 'http://www.wikidata.org/entity/Q1022529', 'http://www.wikidata.org/entity/Q1022535', 'http://www.wikidata.org/entity/Q1022541', 'http://www.wikidata.org/entity/Q102282494', 'http://www.wikidata.org/entity/Q102290707', 'http://www.wikidata.org/entity/Q102291018', 'http://www.wikidata.org/entity/Q1022984', 'http://www.wikidata.org/entity/Q1023044', 'http://www.wikidata.org/entity/Q102312393', 'http://www.wikidata.org/entity/Q1023153', 'http://www.wikidata.org/entity/Q102317', 'http://www.wikidata.org/entity/Q1023290', 'http://www.wikidata.org/entity/Q1023330', 'http://www.wikidata.org/entity/Q1023334', 'http://www.wikidata.org/entity/Q1023359', 'http://www.wikidata.org/entity/Q1023393', 'http://www.wikidata.org/entity/Q1023493', 'http://www.wikidata.org/entity/Q102350', 'http://www.wikidata.org/entity/Q1023521', 'http://www.wikidata.org/entity/Q1023540', 'http://www.wikidata.org/entity/Q102355646', 'http://www.wikidata.org/entity/Q1023619', 'http://www.wikidata.org/entity/Q1023631', 'http://www.wikidata.org/entity/Q1023655', 'http://www.wikidata.org/entity/Q1023691', 'http://www.wikidata.org/entity/Q1023693', 'http://www.wikidata.org/entity/Q1023703', 'http://www.wikidata.org/entity/Q1023712', 'http://www.wikidata.org/entity/Q1023713', 'http://www.wikidata.org/entity/Q1023718', 'http://www.wikidata.org/entity/Q1023720', 'http://www.wikidata.org/entity/Q1023722', 'http://www.wikidata.org/entity/Q1023746', 'http://www.wikidata.org/entity/Q1023760', 'http://www.wikidata.org/entity/Q102397', 'http://www.wikidata.org/entity/Q1024089', 'http://www.wikidata.org/entity/Q1024157', 'http://www.wikidata.org/entity/Q102428504', 'http://www.wikidata.org/entity/Q1024647', 'http://www.wikidata.org/entity/Q1024653', 'http://www.wikidata.org/entity/Q1024667', 'http://www.wikidata.org/entity/Q1024671', 'http://www.wikidata.org/entity/Q1024673', 'http://www.wikidata.org/entity/Q1024676', 'http://www.wikidata.org/entity/Q102469', 'http://www.wikidata.org/entity/Q1024728', 'http://www.wikidata.org/entity/Q1024731', 'http://www.wikidata.org/entity/Q1024793', 'http://www.wikidata.org/entity/Q1025283', 'http://www.wikidata.org/entity/Q1025286', 'http://www.wikidata.org/entity/Q1025299', 'http://www.wikidata.org/entity/Q1025302', 'http://www.wikidata.org/entity/Q1025304', 'http://www.wikidata.org/entity/Q1025309', 'http://www.wikidata.org/entity/Q1025311', 'http://www.wikidata.org/entity/Q1025316', 'http://www.wikidata.org/entity/Q1025320', 'http://www.wikidata.org/entity/Q1025330', 'http://www.wikidata.org/entity/Q1025336', 'http://www.wikidata.org/entity/Q1025396', 'http://www.wikidata.org/entity/Q1025462', 'http://www.wikidata.org/entity/Q1025468', 'http://www.wikidata.org/entity/Q1025475', 'http://www.wikidata.org/entity/Q1025501', 'http://www.wikidata.org/entity/Q1025531', 'http://www.wikidata.org/entity/Q1025577', 'http://www.wikidata.org/entity/Q1025587', 'http://www.wikidata.org/entity/Q1025621', 'http://www.wikidata.org/entity/Q1025625', 'http://www.wikidata.org/entity/Q1025701', 'http://www.wikidata.org/entity/Q1025799', 'http://www.wikidata.org/entity/Q1025801', 'http://www.wikidata.org/entity/Q1025805', 'http://www.wikidata.org/entity/Q1025830', 'http://www.wikidata.org/entity/Q1025861', 'http://www.wikidata.org/entity/Q1025873', 'http://www.wikidata.org/entity/Q1025875', 'http://www.wikidata.org/entity/Q1026057', 'http://www.wikidata.org/entity/Q1026135', 'http://www.wikidata.org/entity/Q1026180', 'http://www.wikidata.org/entity/Q1026185', 'http://www.wikidata.org/entity/Q1026219', 'http://www.wikidata.org/entity/Q1026224', 'http://www.wikidata.org/entity/Q1026244', 'http://www.wikidata.org/entity/Q1026253', 'http://www.wikidata.org/entity/Q1026256', 'http://www.wikidata.org/entity/Q1026270', 'http://www.wikidata.org/entity/Q1026281', 'http://www.wikidata.org/entity/Q1026284', 'http://www.wikidata.org/entity/Q1026296', 'http://www.wikidata.org/entity/Q1026312', 'http://www.wikidata.org/entity/Q1026347', 'http://www.wikidata.org/entity/Q1026436', 'http://www.wikidata.org/entity/Q1026567', 'http://www.wikidata.org/entity/Q1026613', 'http://www.wikidata.org/entity/Q1026616', 'http://www.wikidata.org/entity/Q1026627', 'http://www.wikidata.org/entity/Q1026631', 'http://www.wikidata.org/entity/Q1026633', 'http://www.wikidata.org/entity/Q102682', 'http://www.wikidata.org/entity/Q1026821', 'http://www.wikidata.org/entity/Q1026833', 'http://www.wikidata.org/entity/Q1026971', 'http://www.wikidata.org/entity/Q1026976', 'http://www.wikidata.org/entity/Q1026982', 'http://www.wikidata.org/entity/Q1026987', 'http://www.wikidata.org/entity/Q1026991', 'http://www.wikidata.org/entity/Q1027004', 'http://www.wikidata.org/entity/Q1027041', 'http://www.wikidata.org/entity/Q1027045', 'http://www.wikidata.org/entity/Q1027111', 'http://www.wikidata.org/entity/Q10271130', 'http://www.wikidata.org/entity/Q1027142', 'http://www.wikidata.org/entity/Q1027174', 'http://www.wikidata.org/entity/Q1027188', 'http://www.wikidata.org/entity/Q102737', 'http://www.wikidata.org/entity/Q1027526', 'http://www.wikidata.org/entity/Q1027623', 'http://www.wikidata.org/entity/Q1027828', 'http://www.wikidata.org/entity/Q1027843', 'http://www.wikidata.org/entity/Q1028011', 'http://www.wikidata.org/entity/Q10280269', 'http://www.wikidata.org/entity/Q1028027', 'http://www.wikidata.org/entity/Q1028279', 'http://www.wikidata.org/entity/Q1028289', 'http://www.wikidata.org/entity/Q1029634', 'http://www.wikidata.org/entity/Q1029645', 'http://www.wikidata.org/entity/Q1029650', 'http://www.wikidata.org/entity/Q1029787', 'http://www.wikidata.org/entity/Q1030076', 'http://www.wikidata.org/entity/Q10301027', 'http://www.wikidata.org/entity/Q10301045', 'http://www.wikidata.org/entity/Q103011', 'http://www.wikidata.org/entity/Q1030194', 'http://www.wikidata.org/entity/Q1030202', 'http://www.wikidata.org/entity/Q10306899', 'http://www.wikidata.org/entity/Q10316445', 'http://www.wikidata.org/entity/Q103217', 'http://www.wikidata.org/entity/Q10323671', 'http://www.wikidata.org/entity/Q10327461', 'http://www.wikidata.org/entity/Q1033066', 'http://www.wikidata.org/entity/Q1034159', 'http://www.wikidata.org/entity/Q10344168', 'http://www.wikidata.org/entity/Q1035471', 'http://www.wikidata.org/entity/Q10355792', 'http://www.wikidata.org/entity/Q1036082', 'http://www.wikidata.org/entity/Q10364660', 'http://www.wikidata.org/entity/Q103717', 'http://www.wikidata.org/entity/Q103725', 'http://www.wikidata.org/entity/Q10373307', 'http://www.wikidata.org/entity/Q10378793', 'http://www.wikidata.org/entity/Q10382434', 'http://www.wikidata.org/entity/Q1038323', 'http://www.wikidata.org/entity/Q10387515', 'http://www.wikidata.org/entity/Q103892', 'http://www.wikidata.org/entity/Q10390786', 'http://www.wikidata.org/entity/Q10394607', 'http://www.wikidata.org/entity/Q10396595', 'http://www.wikidata.org/entity/Q10401099', 'http://www.wikidata.org/entity/Q104050371', 'http://www.wikidata.org/entity/Q104302', 'http://www.wikidata.org/entity/Q1043575', 'http://www.wikidata.org/entity/Q1044225', 'http://www.wikidata.org/entity/Q1044689', 'http://www.wikidata.org/entity/Q104591642', 'http://www.wikidata.org/entity/Q104654963', 'http://www.wikidata.org/entity/Q104656158', 'http://www.wikidata.org/entity/Q104656674', 'http://www.wikidata.org/entity/Q104657473', 'http://www.wikidata.org/entity/Q104657987', 'http://www.wikidata.org/entity/Q104658082', 'http://www.wikidata.org/entity/Q104658251', 'http://www.wikidata.org/entity/Q104658390', 'http://www.wikidata.org/entity/Q104658393', 'http://www.wikidata.org/entity/Q104658775', 'http://www.wikidata.org/entity/Q104658935', 'http://www.wikidata.org/entity/Q104658950', 'http://www.wikidata.org/entity/Q1046653', 'http://www.wikidata.org/entity/Q104665636', 'http://www.wikidata.org/entity/Q104670297', 'http://www.wikidata.org/entity/Q104670310', 'http://www.wikidata.org/entity/Q104670333', 'http://www.wikidata.org/entity/Q104670336', 'http://www.wikidata.org/entity/Q104670404', 'http://www.wikidata.org/entity/Q104670507', 'http://www.wikidata.org/entity/Q104670560', 'http://www.wikidata.org/entity/Q104670567', 'http://www.wikidata.org/entity/Q104670572', 'http://www.wikidata.org/entity/Q104670802', 'http://www.wikidata.org/entity/Q104670836', 'http://www.wikidata.org/entity/Q104670943', 'http://www.wikidata.org/entity/Q104670989', 'http://www.wikidata.org/entity/Q104671210', 'http://www.wikidata.org/entity/Q104671410', 'http://www.wikidata.org/entity/Q104671462', 'http://www.wikidata.org/entity/Q104679971', 'http://www.wikidata.org/entity/Q104680188', 'http://www.wikidata.org/entity/Q104712', 'http://www.wikidata.org/entity/Q104713256', 'http://www.wikidata.org/entity/Q104717406', 'http://www.wikidata.org/entity/Q104720', 'http://www.wikidata.org/entity/Q104725', 'http://www.wikidata.org/entity/Q104731', 'http://www.wikidata.org/entity/Q104740', 'http://www.wikidata.org/entity/Q1047734', 'http://www.wikidata.org/entity/Q10480578', 'http://www.wikidata.org/entity/Q1048147', 'http://www.wikidata.org/entity/Q104861662', 'http://www.wikidata.org/entity/Q10498783', 'http://www.wikidata.org/entity/Q1050352', 'http://www.wikidata.org/entity/Q105037', 'http://www.wikidata.org/entity/Q105048', 'http://www.wikidata.org/entity/Q105060', 'http://www.wikidata.org/entity/Q105076326', 'http://www.wikidata.org/entity/Q105084', 'http://www.wikidata.org/entity/Q10509', 'http://www.wikidata.org/entity/Q1051750', 'http://www.wikidata.org/entity/Q10518562', 'http://www.wikidata.org/entity/Q1051957', 'http://www.wikidata.org/entity/Q1052560', 'http://www.wikidata.org/entity/Q105336395', 'http://www.wikidata.org/entity/Q105358597', 'http://www.wikidata.org/entity/Q105358598', 'http://www.wikidata.org/entity/Q105358600', 'http://www.wikidata.org/entity/Q105358605', 'http://www.wikidata.org/entity/Q105392233', 'http://www.wikidata.org/entity/Q105392236', 'http://www.wikidata.org/entity/Q105409933', 'http://www.wikidata.org/entity/Q1054127', 'http://www.wikidata.org/entity/Q1054191', 'http://www.wikidata.org/entity/Q10542373', 'http://www.wikidata.org/entity/Q10543698', 'http://www.wikidata.org/entity/Q10564056', 'http://www.wikidata.org/entity/Q10566', 'http://www.wikidata.org/entity/Q1057594', 'http://www.wikidata.org/entity/Q10587563', 'http://www.wikidata.org/entity/Q105908755', 'http://www.wikidata.org/entity/Q105970025', 'http://www.wikidata.org/entity/Q10600392', 'http://www.wikidata.org/entity/Q10600995', 'http://www.wikidata.org/entity/Q106046148', 'http://www.wikidata.org/entity/Q1060628', 'http://www.wikidata.org/entity/Q106095709', 'http://www.wikidata.org/entity/Q106095820', 'http://www.wikidata.org/entity/Q106095944', 'http://www.wikidata.org/entity/Q106100847', 'http://www.wikidata.org/entity/Q106101158', 'http://www.wikidata.org/entity/Q106115', 'http://www.wikidata.org/entity/Q106122', 'http://www.wikidata.org/entity/Q1061665', 'http://www.wikidata.org/entity/Q1061677', 'http://www.wikidata.org/entity/Q10623109', 'http://www.wikidata.org/entity/Q1062370', 'http://www.wikidata.org/entity/Q1062463', 'http://www.wikidata.org/entity/Q1062635', 'http://www.wikidata.org/entity/Q106274', 'http://www.wikidata.org/entity/Q106285411', 'http://www.wikidata.org/entity/Q10637941', 'http://www.wikidata.org/entity/Q106510487', 'http://www.wikidata.org/entity/Q106581522', 'http://www.wikidata.org/entity/Q106583', 'http://www.wikidata.org/entity/Q10661956', 'http://www.wikidata.org/entity/Q1067163', 'http://www.wikidata.org/entity/Q1067182', 'http://www.wikidata.org/entity/Q1067293', 'http://www.wikidata.org/entity/Q1067464', 'http://www.wikidata.org/entity/Q106849514', 'http://www.wikidata.org/entity/Q10686', 'http://www.wikidata.org/entity/Q106869611', 'http://www.wikidata.org/entity/Q106896', 'http://www.wikidata.org/entity/Q10690', 'http://www.wikidata.org/entity/Q106904207', 'http://www.wikidata.org/entity/Q106914446', 'http://www.wikidata.org/entity/Q1069385', 'http://www.wikidata.org/entity/Q1069835', 'http://www.wikidata.org/entity/Q1070', 'http://www.wikidata.org/entity/Q107013371', 'http://www.wikidata.org/entity/Q1070175', 'http://www.wikidata.org/entity/Q107024198', 'http://www.wikidata.org/entity/Q107094', 'http://www.wikidata.org/entity/Q107106', 'http://www.wikidata.org/entity/Q1071519', 'http://www.wikidata.org/entity/Q10717', 'http://www.wikidata.org/entity/Q107173751', 'http://www.wikidata.org/entity/Q1071771', 'http://www.wikidata.org/entity/Q1072210', 'http://www.wikidata.org/entity/Q1072833', 'http://www.wikidata.org/entity/Q10731600', 'http://www.wikidata.org/entity/Q107398', 'http://www.wikidata.org/entity/Q10743', 'http://www.wikidata.org/entity/Q1074444', 'http://www.wikidata.org/entity/Q1074598', 'http://www.wikidata.org/entity/Q1074644', 'http://www.wikidata.org/entity/Q1074915', 'http://www.wikidata.org/entity/Q1075086', 'http://www.wikidata.org/entity/Q107527228', 'http://www.wikidata.org/entity/Q1075566', 'http://www.wikidata.org/entity/Q1075607', 'http://www.wikidata.org/entity/Q107658630', 'http://www.wikidata.org/entity/Q1076707', 'http://www.wikidata.org/entity/Q10769100', 'http://www.wikidata.org/entity/Q10779', 'http://www.wikidata.org/entity/Q10803523', 'http://www.wikidata.org/entity/Q108036365', 'http://www.wikidata.org/entity/Q108037197', 'http://www.wikidata.org/entity/Q108103451', 'http://www.wikidata.org/entity/Q108103556', 'http://www.wikidata.org/entity/Q108114535', 'http://www.wikidata.org/entity/Q108114607', 'http://www.wikidata.org/entity/Q108114814', 'http://www.wikidata.org/entity/Q108124174', 'http://www.wikidata.org/entity/Q1081284', 'http://www.wikidata.org/entity/Q108133113', 'http://www.wikidata.org/entity/Q108145158', 'http://www.wikidata.org/entity/Q108147538', 'http://www.wikidata.org/entity/Q108150764', 'http://www.wikidata.org/entity/Q1081635', 'http://www.wikidata.org/entity/Q108166787', 'http://www.wikidata.org/entity/Q108208234', 'http://www.wikidata.org/entity/Q108208378', 'http://www.wikidata.org/entity/Q108209953', 'http://www.wikidata.org/entity/Q108223', 'http://www.wikidata.org/entity/Q108223053', 'http://www.wikidata.org/entity/Q108227837', 'http://www.wikidata.org/entity/Q108228329', 'http://www.wikidata.org/entity/Q108239161', 'http://www.wikidata.org/entity/Q10824077', 'http://www.wikidata.org/entity/Q108248706', 'http://www.wikidata.org/entity/Q108250894', 'http://www.wikidata.org/entity/Q108254387', 'http://www.wikidata.org/entity/Q108254637', 'http://www.wikidata.org/entity/Q108266881', 'http://www.wikidata.org/entity/Q108293179', 'http://www.wikidata.org/entity/Q1083', 'http://www.wikidata.org/entity/Q108301469', 'http://www.wikidata.org/entity/Q10837783', 'http://www.wikidata.org/entity/Q10839880', 'http://www.wikidata.org/entity/Q10842552', 'http://www.wikidata.org/entity/Q10853792', 'http://www.wikidata.org/entity/Q108554160', 'http://www.wikidata.org/entity/Q10859337', 'http://www.wikidata.org/entity/Q10859501', 'http://www.wikidata.org/entity/Q10860440', 'http://www.wikidata.org/entity/Q10861438', 'http://www.wikidata.org/entity/Q108672', 'http://www.wikidata.org/entity/Q10867816', 'http://www.wikidata.org/entity/Q108679', 'http://www.wikidata.org/entity/Q108682025', 'http://www.wikidata.org/entity/Q108750045', 'http://www.wikidata.org/entity/Q108777536', 'http://www.wikidata.org/entity/Q1087848', 'http://www.wikidata.org/entity/Q10878511', 'http://www.wikidata.org/entity/Q108830442', 'http://www.wikidata.org/entity/Q10885263', 'http://www.wikidata.org/entity/Q1088760', 'http://www.wikidata.org/entity/Q108886420', 'http://www.wikidata.org/entity/Q1089052', 'http://www.wikidata.org/entity/Q108908310', 'http://www.wikidata.org/entity/Q10891328', 'http://www.wikidata.org/entity/Q1089449', 'http://www.wikidata.org/en</t>
-  </si>
-  <si>
-    <t>Give me the capitals of all countries that the Himalayas run through.</t>
-  </si>
-  <si>
-    <t>['http://www.wikidata.org/entity/Q1362', 'http://www.wikidata.org/entity/Q3037', 'http://www.wikidata.org/entity/Q37400', 'http://www.wikidata.org/entity/Q5838', 'http://www.wikidata.org/entity/Q9270', 'http://www.wikidata.org/entity/Q956', 'http://www.wikidata.org/entity/Q987']</t>
-  </si>
-  <si>
-    <t>['http://www.wikidata.org/entity/Q2807']</t>
-  </si>
-  <si>
-    <t>how much is the population Iraq?</t>
-  </si>
-  <si>
-    <t>['38274618']</t>
-  </si>
-  <si>
-    <t>['67326569']</t>
-  </si>
-  <si>
-    <t>What is the capital of Canada?</t>
-  </si>
-  <si>
-    <t>['http://www.wikidata.org/entity/Q1930']</t>
-  </si>
-  <si>
-    <t>['http://www.wikidata.org/entity/Q61']</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -105,43 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -429,86 +420,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="241.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="255.77734375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>question</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>expected_answers</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>lama_answers</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>is_correct</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Which city has the least inhabitants?</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q2590944']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1000333', 'http://www.wikidata.org/entity/Q1000341', 'http://www.wikidata.org/entity/Q1000346', 'http://www.wikidata.org/entity/Q1000438', 'http://www.wikidata.org/entity/Q10006', 'http://www.wikidata.org/entity/Q1000839', 'http://www.wikidata.org/entity/Q1000844', 'http://www.wikidata.org/entity/Q1000883', 'http://www.wikidata.org/entity/Q1000887', 'http://www.wikidata.org/entity/Q1000938', 'http://www.wikidata.org/entity/Q1001200', 'http://www.wikidata.org/entity/Q1001307', 'http://www.wikidata.org/entity/Q1001322', 'http://www.wikidata.org/entity/Q10014', 'http://www.wikidata.org/entity/Q1001440', 'http://www.wikidata.org/entity/Q1001496', 'http://www.wikidata.org/entity/Q1001517', 'http://www.wikidata.org/entity/Q1001522', 'http://www.wikidata.org/entity/Q1001571', 'http://www.wikidata.org/entity/Q1001817', 'http://www.wikidata.org/entity/Q100188', 'http://www.wikidata.org/entity/Q1001887', 'http://www.wikidata.org/entity/Q1001897', 'http://www.wikidata.org/entity/Q1001914', 'http://www.wikidata.org/entity/Q1001941', 'http://www.wikidata.org/entity/Q1001959', 'http://www.wikidata.org/entity/Q1002035', 'http://www.wikidata.org/entity/Q1002052', 'http://www.wikidata.org/entity/Q1002144', 'http://www.wikidata.org/entity/Q1002286', 'http://www.wikidata.org/entity/Q1002533', 'http://www.wikidata.org/entity/Q1002557', 'http://www.wikidata.org/entity/Q1002560', 'http://www.wikidata.org/entity/Q1002638', 'http://www.wikidata.org/entity/Q1002658', 'http://www.wikidata.org/entity/Q1002670', 'http://www.wikidata.org/entity/Q1002685', 'http://www.wikidata.org/entity/Q1002696', 'http://www.wikidata.org/entity/Q1002807', 'http://www.wikidata.org/entity/Q1002900', 'http://www.wikidata.org/entity/Q1002944', 'http://www.wikidata.org/entity/Q1003016', 'http://www.wikidata.org/entity/Q1003112', 'http://www.wikidata.org/entity/Q1003264', 'http://www.wikidata.org/entity/Q1003267', 'http://www.wikidata.org/entity/Q1003272', 'http://www.wikidata.org/entity/Q1003276', 'http://www.wikidata.org/entity/Q1003279', 'http://www.wikidata.org/entity/Q1003283', 'http://www.wikidata.org/entity/Q1003318', 'http://www.wikidata.org/entity/Q1003903', 'http://www.wikidata.org/entity/Q1004283', 'http://www.wikidata.org/entity/Q1004290', 'http://www.wikidata.org/entity/Q1004295', 'http://www.wikidata.org/entity/Q1004298', 'http://www.wikidata.org/entity/Q1004302', 'http://www.wikidata.org/entity/Q1004312', 'http://www.wikidata.org/entity/Q1004320', 'http://www.wikidata.org/entity/Q1004328', 'http://www.wikidata.org/entity/Q10045', 'http://www.wikidata.org/entity/Q1004686', 'http://www.wikidata.org/entity/Q1004716', 'http://www.wikidata.org/entity/Q1004822', 'http://www.wikidata.org/entity/Q10052', 'http://www.wikidata.org/entity/Q1005350', 'http://www.wikidata.org/entity/Q1005356', 'http://www.wikidata.org/entity/Q1005359', 'http://www.wikidata.org/entity/Q1005384', 'http://www.wikidata.org/entity/Q1005394', 'http://www.wikidata.org/entity/Q1005403', 'http://www.wikidata.org/entity/Q1005409', 'http://www.wikidata.org/entity/Q1005414', 'http://www.wikidata.org/entity/Q1005419', 'http://www.wikidata.org/entity/Q1005428', 'http://www.wikidata.org/entity/Q1005435', 'http://www.wikidata.org/entity/Q1005442', 'http://www.wikidata.org/entity/Q1005453', 'http://www.wikidata.org/entity/Q1005464', 'http://www.wikidata.org/entity/Q1005472', 'http://www.wikidata.org/entity/Q1005483', 'http://www.wikidata.org/entity/Q1005492', 'http://www.wikidata.org/entity/Q1005503', 'http://www.wikidata.org/entity/Q1005511', 'http://www.wikidata.org/entity/Q1005538', 'http://www.wikidata.org/entity/Q1005725', 'http://www.wikidata.org/entity/Q1005770', 'http://www.wikidata.org/entity/Q1005827', 'http://www.wikidata.org/entity/Q1005837', 'http://www.wikidata.org/entity/Q1005855', 'http://www.wikidata.org/entity/Q1005885', 'http://www.wikidata.org/entity/Q1005905', 'http://www.wikidata.org/entity/Q1005972', 'http://www.wikidata.org/entity/Q1006081', 'http://www.wikidata.org/entity/Q1006155', 'http://www.wikidata.org/entity/Q1006165', 'http://www.wikidata.org/entity/Q1006240', 'http://www.wikidata.org/entity/Q1006277', 'http://www.wikidata.org/entity/Q1006296', 'http://www.wikidata.org/entity/Q1006303', 'http://www.wikidata.org/entity/Q1006321', 'http://www.wikidata.org/entity/Q1006343', 'http://www.wikidata.org/entity/Q1006764', 'http://www.wikidata.org/entity/Q1006772', 'http://www.wikidata.org/entity/Q1006788', 'http://www.wikidata.org/entity/Q1006813', 'http://www.wikidata.org/entity/Q1007232', 'http://www.wikidata.org/entity/Q1007342', 'http://www.wikidata.org/entity/Q1007355', 'http://www.wikidata.org/entity/Q1007407', 'http://www.wikidata.org/entity/Q1007479', 'http://www.wikidata.org/entity/Q1007634', 'http://www.wikidata.org/entity/Q1007647', 'http://www.wikidata.org/entity/Q1007702', 'http://www.wikidata.org/entity/Q1007719', 'http://www.wikidata.org/entity/Q1008390', 'http://www.wikidata.org/entity/Q1008456', 'http://www.wikidata.org/entity/Q1008761', 'http://www.wikidata.org/entity/Q1008853', 'http://www.wikidata.org/entity/Q1009161', 'http://www.wikidata.org/entity/Q1009253', 'http://www.wikidata.org/entity/Q1009308', 'http://www.wikidata.org/entity/Q1009509', 'http://www.wikidata.org/entity/Q1009549', 'http://www.wikidata.org/entity/Q1010', 'http://www.wikidata.org/entity/Q1010153', 'http://www.wikidata.org/entity/Q1010278', 'http://www.wikidata.org/entity/Q1010367', 'http://www.wikidata.org/entity/Q1010816', 'http://www.wikidata.org/entity/Q1010954', 'http://www.wikidata.org/entity/Q1010960', 'http://www.wikidata.org/entity/Q1010979', 'http://www.wikidata.org/entity/Q1010985', 'http://www.wikidata.org/entity/Q1011011', 'http://www.wikidata.org/entity/Q1011016', 'http://www.wikidata.org/entity/Q1011047', 'http://www.wikidata.org/entity/Q101145616', 'http://www.wikidata.org/entity/Q1011488', 'http://www.wikidata.org/entity/Q1011553', 'http://www.wikidata.org/entity/Q1011863', 'http://www.wikidata.org/entity/Q1011873', 'http://www.wikidata.org/entity/Q1011882', 'http://www.wikidata.org/entity/Q1011890', 'http://www.wikidata.org/entity/Q1011972', 'http://www.wikidata.org/entity/Q1012', 'http://www.wikidata.org/entity/Q101254', 'http://www.wikidata.org/entity/Q1012828', 'http://www.wikidata.org/entity/Q1012831', 'http://www.wikidata.org/entity/Q1012862', 'http://www.wikidata.org/entity/Q1012868', 'http://www.wikidata.org/entity/Q1012881', 'http://www.wikidata.org/entity/Q1012887', 'http://www.wikidata.org/entity/Q1012924', 'http://www.wikidata.org/entity/Q1013119', 'http://www.wikidata.org/entity/Q1013379', 'http://www.wikidata.org/entity/Q1013424', 'http://www.wikidata.org/entity/Q1013428', 'http://www.wikidata.org/entity/Q1013454', 'http://www.wikidata.org/entity/Q1013526', 'http://www.wikidata.org/entity/Q1014010', 'http://www.wikidata.org/entity/Q101418', 'http://www.wikidata.org/entity/Q1014231', 'http://www.wikidata.org/entity/Q1014235', 'http://www.wikidata.org/entity/Q1014248', 'http://www.wikidata.org/entity/Q1014285', 'http://www.wikidata.org/entity/Q1014306', 'http://www.wikidata.org/entity/Q1014315', 'http://www.wikidata.org/entity/Q1014367', 'http://www.wikidata.org/entity/Q1014375', 'http://www.wikidata.org/entity/Q1014380', 'http://www.wikidata.org/entity/Q1014430', 'http://www.wikidata.org/entity/Q1014433', 'http://www.wikidata.org/entity/Q1014456', 'http://www.wikidata.org/entity/Q1014474', 'http://www.wikidata.org/entity/Q1014481', 'http://www.wikidata.org/entity/Q1014493', 'http://www.wikidata.org/entity/Q1014504', 'http://www.wikidata.org/entity/Q1014511', 'http://www.wikidata.org/entity/Q1014530', 'http://www.wikidata.org/entity/Q1014554', 'http://www.wikidata.org/entity/Q1014561', 'http://www.wikidata.org/entity/Q1014564', 'http://www.wikidata.org/entity/Q1015', 'http://www.wikidata.org/entity/Q1015036', 'http://www.wikidata.org/entity/Q1015152', 'http://www.wikidata.org/entity/Q1015160', 'http://www.wikidata.org/entity/Q1015165', 'http://www.wikidata.org/entity/Q1015172', 'http://www.wikidata.org/entity/Q101530', 'http://www.wikidata.org/entity/Q1015472', 'http://www.wikidata.org/entity/Q1015618', 'http://www.wikidata.org/entity/Q1015639', 'http://www.wikidata.org/entity/Q1015672', 'http://www.wikidata.org/entity/Q1015681', 'http://www.wikidata.org/entity/Q1015690', 'http://www.wikidata.org/entity/Q1015699', 'http://www.wikidata.org/entity/Q1015727', 'http://www.wikidata.org/entity/Q1015752', 'http://www.wikidata.org/entity/Q1015773', 'http://www.wikidata.org/entity/Q1015796', 'http://www.wikidata.org/entity/Q1015891', 'http://www.wikidata.org/entity/Q101625', 'http://www.wikidata.org/entity/Q1016289', 'http://www.wikidata.org/entity/Q1016827', 'http://www.wikidata.org/entity/Q1016873', 'http://www.wikidata.org/entity/Q1016881', 'http://www.wikidata.org/entity/Q101704', 'http://www.wikidata.org/entity/Q1017167', 'http://www.wikidata.org/entity/Q1017183', 'http://www.wikidata.org/entity/Q1017208', 'http://www.wikidata.org/entity/Q1017210', 'http://www.wikidata.org/entity/Q1017314', 'http://www.wikidata.org/entity/Q1017331', 'http://www.wikidata.org/entity/Q1017358', 'http://www.wikidata.org/entity/Q1017362', 'http://www.wikidata.org/entity/Q1017387', 'http://www.wikidata.org/entity/Q1017554', 'http://www.wikidata.org/entity/Q1017594', 'http://www.wikidata.org/entity/Q1017624', 'http://www.wikidata.org/entity/Q1017630', 'http://www.wikidata.org/entity/Q1017637', 'http://www.wikidata.org/entity/Q1017644', 'http://www.wikidata.org/entity/Q1017651', 'http://www.wikidata.org/entity/Q1017662', 'http://www.wikidata.org/entity/Q1017673', 'http://www.wikidata.org/entity/Q1017678', 'http://www.wikidata.org/entity/Q1017683', 'http://www.wikidata.org/entity/Q1017691', 'http://www.wikidata.org/entity/Q1017696', 'http://www.wikidata.org/entity/Q1017710', 'http://www.wikidata.org/entity/Q1017735', 'http://www.wikidata.org/entity/Q1017971', 'http://www.wikidata.org/entity/Q1018092', 'http://www.wikidata.org/entity/Q1018116', 'http://www.wikidata.org/entity/Q1018160', 'http://www.wikidata.org/entity/Q1018163', 'http://www.wikidata.org/entity/Q1018167', 'http://www.wikidata.org/entity/Q1018173', 'http://www.wikidata.org/entity/Q1018201', 'http://www.wikidata.org/entity/Q1018215', 'http://www.wikidata.org/entity/Q1018239', 'http://www.wikidata.org/entity/Q1018271', 'http://www.wikidata.org/entity/Q1018369', 'http://www.wikidata.org/entity/Q1018501', 'http://www.wikidata.org/entity/Q1018574', 'http://www.wikidata.org/entity/Q1018584', 'http://www.wikidata.org/entity/Q1018592', 'http://www.wikidata.org/entity/Q1018701', 'http://www.wikidata.org/entity/Q1018781', 'http://www.wikidata.org/entity/Q1018868', 'http://www.wikidata.org/entity/Q1018872', 'http://www.wikidata.org/entity/Q1019060', 'http://www.wikidata.org/entity/Q1019152', 'http://www.wikidata.org/entity/Q1019287', 'http://www.wikidata.org/entity/Q1019356', 'http://www.wikidata.org/entity/Q1019377', 'http://www.wikidata.org/entity/Q1019402', 'http://www.wikidata.org/entity/Q1019405', 'http://www.wikidata.org/entity/Q1019424', 'http://www.wikidata.org/entity/Q1019429', 'http://www.wikidata.org/entity/Q1019443', 'http://www.wikidata.org/entity/Q1019448', 'http://www.wikidata.org/entity/Q1019452', 'http://www.wikidata.org/entity/Q1019466', 'http://www.wikidata.org/entity/Q1019470', 'http://www.wikidata.org/entity/Q1019496', 'http://www.wikidata.org/entity/Q1019505', 'http://www.wikidata.org/entity/Q1019534', 'http://www.wikidata.org/entity/Q1019991', 'http://www.wikidata.org/entity/Q1020010', 'http://www.wikidata.org/entity/Q1020110', 'http://www.wikidata.org/entity/Q1020261', 'http://www.wikidata.org/entity/Q1020263', 'http://www.wikidata.org/entity/Q1020273', 'http://www.wikidata.org/entity/Q1020276', 'http://www.wikidata.org/entity/Q1020279', 'http://www.wikidata.org/entity/Q1020288', 'http://www.wikidata.org/entity/Q1020292', 'http://www.wikidata.org/entity/Q1020297', 'http://www.wikidata.org/entity/Q1020314', 'http://www.wikidata.org/entity/Q1020320', 'http://www.wikidata.org/entity/Q1020338', 'http://www.wikidata.org/entity/Q1020384', 'http://www.wikidata.org/entity/Q1020396', 'http://www.wikidata.org/entity/Q1020477', 'http://www.wikidata.org/entity/Q1020484', 'http://www.wikidata.org/entity/Q1020490', 'http://www.wikidata.org/entity/Q1020535', 'http://www.wikidata.org/entity/Q1020627', 'http://www.wikidata.org/entity/Q1020649', 'http://www.wikidata.org/entity/Q1020762', 'http://www.wikidata.org/entity/Q1020776', 'http://www.wikidata.org/entity/Q1020785', 'http://www.wikidata.org/entity/Q1020794', 'http://www.wikidata.org/entity/Q1020969', 'http://www.wikidata.org/entity/Q1020997', 'http://www.wikidata.org/entity/Q1021', 'http://www.wikidata.org/entity/Q1021013', 'http://www.wikidata.org/entity/Q1021223', 'http://www.wikidata.org/entity/Q1021263', 'http://www.wikidata.org/entity/Q1021272', 'http://www.wikidata.org/entity/Q1021277', 'http://www.wikidata.org/entity/Q1021282', 'http://www.wikidata.org/entity/Q1021286', 'http://www.wikidata.org/entity/Q1021294', 'http://www.wikidata.org/entity/Q1021592', 'http://www.wikidata.org/entity/Q1021638', 'http://www.wikidata.org/entity/Q1021800', 'http://www.wikidata.org/entity/Q1021903', 'http://www.wikidata.org/entity/Q1022131', 'http://www.wikidata.org/entity/Q1022152', 'http://www.wikidata.org/entity/Q1022170', 'http://www.wikidata.org/entity/Q1022481', 'http://www.wikidata.org/entity/Q1022488', 'http://www.wikidata.org/entity/Q1022984', 'http://www.wikidata.org/entity/Q1023044', 'http://www.wikidata.org/entity/Q1023153', 'http://www.wikidata.org/entity/Q102317', 'http://www.wikidata.org/entity/Q1023290', 'http://www.wikidata.org/entity/Q1023330', 'http://www.wikidata.org/entity/Q1023359', 'http://www.wikidata.org/entity/Q1023393', 'http://www.wikidata.org/entity/Q1023493', 'http://www.wikidata.org/entity/Q102350', 'http://www.wikidata.org/entity/Q1023521', 'http://www.wikidata.org/entity/Q1023540', 'http://www.wikidata.org/entity/Q1023619', 'http://www.wikidata.org/entity/Q1023631', 'http://www.wikidata.org/entity/Q1023655', 'http://www.wikidata.org/entity/Q1023693', 'http://www.wikidata.org/entity/Q1023703', 'http://www.wikidata.org/entity/Q1023712', 'http://www.wikidata.org/entity/Q1023713', 'http://www.wikidata.org/entity/Q1023720', 'http://www.wikidata.org/entity/Q1023722', 'http://www.wikidata.org/entity/Q1023746', 'http://www.wikidata.org/entity/Q1023760', 'http://www.wikidata.org/entity/Q102397', 'http://www.wikidata.org/entity/Q1024647', 'http://www.wikidata.org/entity/Q1024653', 'http://www.wikidata.org/entity/Q1024671', 'http://www.wikidata.org/entity/Q1024673', 'http://www.wikidata.org/entity/Q1024676', 'http://www.wikidata.org/entity/Q102469', 'http://www.wikidata.org/entity/Q1024728', 'http://www.wikidata.org/entity/Q1024731', 'http://www.wikidata.org/entity/Q1025283', 'http://www.wikidata.org/entity/Q1025299', 'http://www.wikidata.org/entity/Q1025302', 'http://www.wikidata.org/entity/Q1025304', 'http://www.wikidata.org/entity/Q1025309', 'http://www.wikidata.org/entity/Q1025311', 'http://www.wikidata.org/entity/Q1025316', 'http://www.wikidata.org/entity/Q1025320', 'http://www.wikidata.org/entity/Q1025330', 'http://www.wikidata.org/entity/Q1025336', 'http://www.wikidata.org/entity/Q1025396', 'http://www.wikidata.org/entity/Q1025462', 'http://www.wikidata.org/entity/Q1025468', 'http://www.wikidata.org/entity/Q1025475', 'http://www.wikidata.org/entity/Q1025531', 'http://www.wikidata.org/entity/Q1025587', 'http://www.wikidata.org/entity/Q1025621', 'http://www.wikidata.org/entity/Q1025701', 'http://www.wikidata.org/entity/Q1025799', 'http://www.wikidata.org/entity/Q1025801', 'http://www.wikidata.org/entity/Q1025805', 'http://www.wikidata.org/entity/Q1025830', 'http://www.wikidata.org/entity/Q1025861', 'http://www.wikidata.org/entity/Q1025873', 'http://www.wikidata.org/entity/Q1025875', 'http://www.wikidata.org/entity/Q1026057', 'http://www.wikidata.org/entity/Q1026185', 'http://www.wikidata.org/entity/Q1026219', 'http://www.wikidata.org/entity/Q1026224', 'http://www.wikidata.org/entity/Q1026253', 'http://www.wikidata.org/entity/Q1026256', 'http://www.wikidata.org/entity/Q1026270', 'http://www.wikidata.org/entity/Q1026281', 'http://www.wikidata.org/entity/Q1026284', 'http://www.wikidata.org/entity/Q1026296', 'http://www.wikidata.org/entity/Q1026312', 'http://www.wikidata.org/entity/Q1026436', 'http://www.wikidata.org/entity/Q1026567', 'http://www.wikidata.org/entity/Q1026616', 'http://www.wikidata.org/entity/Q1026631', 'http://www.wikidata.org/entity/Q1026633', 'http://www.wikidata.org/entity/Q102682', 'http://www.wikidata.org/entity/Q1026821', 'http://www.wikidata.org/entity/Q1026971', 'http://www.wikidata.org/entity/Q1026976', 'http://www.wikidata.org/entity/Q1026982', 'http://www.wikidata.org/entity/Q1026987', 'http://www.wikidata.org/entity/Q1026991', 'http://www.wikidata.org/entity/Q1027004', 'http://www.wikidata.org/entity/Q1027041', 'http://www.wikidata.org/entity/Q1027045', 'http://www.wikidata.org/entity/Q1027111', 'http://www.wikidata.org/entity/Q1027142', 'http://www.wikidata.org/entity/Q102737', 'http://www.wikidata.org/entity/Q1027526', 'http://www.wikidata.org/entity/Q1027623', 'http://www.wikidata.org/entity/Q1027843', 'http://www.wikidata.org/entity/Q1028027', 'http://www.wikidata.org/entity/Q1028279', 'http://www.wikidata.org/entity/Q1028289', 'http://www.wikidata.org/entity/Q1029634', 'http://www.wikidata.org/entity/Q1029645', 'http://www.wikidata.org/entity/Q1029650', 'http://www.wikidata.org/entity/Q103011', 'http://www.wikidata.org/entity/Q1030194', 'http://www.wikidata.org/entity/Q103217', 'http://www.wikidata.org/entity/Q10323671', 'http://www.wikidata.org/entity/Q1033066', 'http://www.wikidata.org/entity/Q1034159', 'http://www.wikidata.org/entity/Q1035471', 'http://www.wikidata.org/entity/Q10355792', 'http://www.wikidata.org/entity/Q103717', 'http://www.wikidata.org/entity/Q103725', 'http://www.wikidata.org/entity/Q10373307', 'http://www.wikidata.org/entity/Q10378793', 'http://www.wikidata.org/entity/Q1038323', 'http://www.wikidata.org/entity/Q103892', 'http://www.wikidata.org/entity/Q104050371', 'http://www.wikidata.org/entity/Q104302', 'http://www.wikidata.org/entity/Q1043575', 'http://www.wikidata.org/entity/Q1044225', 'http://www.wikidata.org/entity/Q1044689', 'http://www.wikidata.org/entity/Q1046653', 'http://www.wikidata.org/entity/Q104665636', 'http://www.wikidata.org/entity/Q104712', 'http://www.wikidata.org/entity/Q104720', 'http://www.wikidata.org/entity/Q104725', 'http://www.wikidata.org/entity/Q104731', 'http://www.wikidata.org/entity/Q104740', 'http://www.wikidata.org/entity/Q1047734', 'http://www.wikidata.org/entity/Q1048147', 'http://www.wikidata.org/entity/Q10498783', 'http://www.wikidata.org/entity/Q105037', 'http://www.wikidata.org/entity/Q105048', 'http://www.wikidata.org/entity/Q105060', 'http://www.wikidata.org/entity/Q105084', 'http://www.wikidata.org/entity/Q10509', 'http://www.wikidata.org/entity/Q1051750', 'http://www.wikidata.org/entity/Q10518562', 'http://www.wikidata.org/entity/Q1051957', 'http://www.wikidata.org/entity/Q1052560', 'http://www.wikidata.org/entity/Q1054127', 'http://www.wikidata.org/entity/Q1054191', 'http://www.wikidata.org/entity/Q10566', 'http://www.wikidata.org/entity/Q10587563', 'http://www.wikidata.org/entity/Q10600995', 'http://www.wikidata.org/entity/Q1060628', 'http://www.wikidata.org/entity/Q1061665', 'http://www.wikidata.org/entity/Q1061677', 'http://www.wikidata.org/entity/Q1062370', 'http://www.wikidata.org/entity/Q1062635', 'http://www.wikidata.org/entity/Q106274', 'http://www.wikidata.org/entity/Q106583', 'http://www.wikidata.org/entity/Q10661956', 'http://www.wikidata.org/entity/Q1067163', 'http://www.wikidata.org/entity/Q1067464', 'http://www.wikidata.org/entity/Q10686', 'http://www.wikidata.org/entity/Q106869611', 'http://www.wikidata.org/entity/Q106896', 'http://www.wikidata.org/entity/Q10690', 'http://www.wikidata.org/entity/Q1069385', 'http://www.wikidata.org/entity/Q1069835', 'http://www.wikidata.org/entity/Q1070', 'http://www.wikidata.org/entity/Q1070175', 'http://www.wikidata.org/entity/Q107094', 'http://www.wikidata.org/entity/Q107106', 'http://www.wikidata.org/entity/Q10717', 'http://www.wikidata.org/entity/Q1071771', 'http://www.wikidata.org/entity/Q1072833', 'http://www.wikidata.org/entity/Q107398', 'http://www.wikidata.org/entity/Q10743', 'http://www.wikidata.org/entity/Q1074444', 'http://www.wikidata.org/entity/Q1075086', 'http://www.wikidata.org/entity/Q107527228', 'http://www.wikidata.org/entity/Q1075566', 'http://www.wikidata.org/entity/Q1075607', 'http://www.wikidata.org/entity/Q10779', 'http://www.wikidata.org/entity/Q1081635', 'http://www.wikidata.org/entity/Q108223', 'http://www.wikidata.org/entity/Q1083', 'http://www.wikidata.org/entity/Q10837783', 'http://www.wikidata.org/entity/Q10853792', 'http://www.wikidata.org/entity/Q10859337', 'http://www.wikidata.org/entity/Q10859501', 'http://www.wikidata.org/entity/Q108672', 'http://www.wikidata.org/entity/Q108679', 'http://www.wikidata.org/entity/Q1088760', 'http://www.wikidata.org/entity/Q1089052', 'http://www.wikidata.org/entity/Q108908310', 'http://www.wikidata.org/entity/Q1090858', 'http://www.wikidata.org/entity/Q109092', 'http://www.wikidata.org/entity/Q1093448', 'http://www.wikidata.org/entity/Q1093479', 'http://www.wikidata.org/entity/Q109386', 'http://www.wikidata.org/entity/Q1094355', 'http://www.wikidata.org/entity/Q1094372', 'http://www.wikidata.org/entity/Q109494', 'http://www.wikidata.org/entity/Q109535', 'http://www.wikidata.org/entity/Q109548535', 'http://www.wikidata.org/entity/Q109949', 'http://www.wikidata.org/entity/Q110011', 'http://www.wikidata.org/entity/Q1100303', 'http://www.wikidata.org/entity/Q11004410', 'http://www.wikidata.org/entity/Q1100543', 'http://www.wikidata.org/entity/Q11010032', 'http://www.wikidata.org/entity/Q1102140', 'http://www.wikidata.org/entity/Q110218', 'http://www.wikidata.org/entity/Q1102546', 'http://www.wikidata.org/entity/Q1102602', 'http://www.wikidata.org/entity/Q1104010', 'http://www.wikidata.org/entity/Q11041865', 'http://www.wikidata.org/entity/Q11043', 'http://www.wikidata.org/entity/Q110732', 'http://www.wikidata.org/entity/Q1110026', 'http://www.wikidata.org/entity/Q1110037', 'http://www.wikidata.org/entity/Q1111957', 'http://www.wikidata.org/entity/Q1113311', 'http://www.wikidata.org/entity/Q1115195', 'http://www.wikidata.org/entity/Q11160662', 'http://www.wikidata.org/entity/Q111607005', 'http://www.wikidata.org/entity/Q11168982', 'http://www.wikidata.org/entity/Q1117303', 'http://www.wikidata.org/entity/Q11194', 'http://www.wikidata.org/entity/Q11198998', 'http://www.wikidata.org/entity/Q1120810', 'http://www.wikidata.org/entity/Q1120978', 'http://www.wikidata.org/entity/Q1122800', 'http://www.wikidata.org/entity/Q11249733', 'http://www.wikidata.org/entity/Q112657', 'http://www.wikidata.org/entity/Q112817', 'http://www.wikidata.org/entity/Q11285', 'http://www.wikidata.org/entity/Q1130843', 'http://www.wikidata.org/entity/Q1134454', 'http://www.wikidata.org/entity/Q113464', 'http://www.wikidata.org/entity/Q1136023', 'http://www.wikidata.org/entity/Q1136771', 'http://www.wikidata.org/entity/Q1140136', 'http://www.wikidata.org/entity/Q114093', 'http://www.wikidata.org/entity/Q1141853', 'http://www.wikidata.org/entity/Q1141858', 'http://www.wikidata.org/entity/Q114257', 'http://www.wikidata.org/entity/Q1142926', 'http://www.wikidata.org/entity/Q1143259', 'http://www.wikidata.org/entity/Q1146939', 'http://www.wikidata.org/entity/Q1149495', 'http://www.wikidata.org/entity/Q1149502', 'http://www.wikidata.org/entity/Q114970', 'http://www.wikidata.org/entity/Q114977', 'http://www.wikidata.org/entity/Q114984', 'http://www.wikidata.org/entity/Q115006', 'http://www.wikidata.org/entity/Q1150271', 'http://www.wikidata.org/entity/Q115045527', 'http://www.wikidata.org/entity/Q115256', 'http://www.wikidata.org/entity/Q115276', 'http://www.wikidata.org/entity/Q115323', 'http://www.wikidata.org/entity/Q115329', 'http://www.wikidata.org/entity/Q115382', 'http://www.wikidata.org/entity/Q1154', 'http://www.wikidata.org/entity/Q115403', 'http://www.wikidata.org/entity/Q115465', 'http://www.wikidata.org/entity/Q1156', 'http://www.wikidata.org/entity/Q11568', 'http://www.wikidata.org/entity/Q1159408', 'http://www.wikidata.org/entity/Q116156', 'http://www.wikidata.org/entity/Q116341', 'http://www.wikidata.org/entity/Q116423012', 'http://www.wikidata.org/entity/Q116450456', 'http://www.wikidata.org/entity/Q116524', 'http://www.wikidata.org/entity/Q1166791', 'http://www.wikidata.org/entity/Q116813782', 'http://www.wikidata.org/entity/Q1170305', 'http://www.wikidata.org/entity/Q117040', 'http://www.wikidata.org/entity/Q11725', 'http://www.wikidata.org/entity/Q1173008', 'http://www.wikidata.org/entity/Q11736', 'http://www.wikidata.org/entity/Q11739', 'http://www.wikidata.org/entity/Q117625', 'http://www.wikidata.org/entity/Q11792967', 'http://www.wikidata.org/entity/Q1179634', 'http://www.wikidata.org/entity/Q1179844', 'http://www.wikidata.org/entity/Q118174166', 'http://www.wikidata.org/entity/Q1182807', 'http://www.wikidata.org/entity/Q118366736', 'http://www.wikidata.org/entity/Q118434309', 'http://www.wikidata.org/entity/Q1185115', 'http://www.wikidata.org/entity/Q11854', 'http://www.wikidata.org/entity/Q11864', 'http://www.wikidata.org/entity/Q1188560', 'http://www.wikidata.org/entity/Q118910', 'http://www.wikidata.org/entity/Q118995', 'http://www.wikidata.org/entity/Q1189982', 'http://www.wikidata.org/entity/Q1190869', 'http://www.wikidata.org/entity/Q11909', 'http://www.wikidata.org/entity/Q11910', 'http://www.wikidata.org/entity/Q1191011', 'http://www.wikidata.org/entity/Q1192453', 'http://www.wikidata.org/entity/Q1192513', 'http://www.wikidata.org/entity/Q1193830', 'http://www.wikidata.org/entity/Q11938328', 'http://www.wikidata.org/entity/Q1195207', 'http://www.wikidata.org/entity/Q11959', 'http://www.wikidata.org/entity/Q1195983', 'http://www.wikidata.org/entity/Q1196877', 'http://www.wikidata.org/entity/Q11977', 'http://www.wikidata.org/entity/Q119806208', 'http://www.wikidata.org/entity/Q11994', 'http://www.wikidata.org/entity/Q12004287', 'http://www.wikidata.org/entity/Q1202229', 'http://www.wikidata.org/entity/Q1203781', 'http://www.wikidata.org/entity/Q12059689', 'http://www.wikidata.org/entity/Q1208152', 'http://www.wikidata.org/entity/Q1209397', 'http://www.wikidata.org/entity/Q1209404', 'http://www.wikidata.org/entity/Q1210015', 'http://www.wikidata.org/entity/Q121074736', 'http://www.wikidata.org/entity/Q121150916', 'http://www.wikidata.org/entity/Q1218', 'http://www.wikidata.org/entity/Q12184496', 'http://www.wikidata.org/entity/Q12185451', 'http://www.wikidata.org/entity/Q12185628', 'http://www.wikidata.org/entity/Q12186298', 'http://www.wikidata.org/entity/Q12186493', 'http://www.wikidata.org/entity/Q12186928', 'http://www.wikidata.org/entity/Q12187525', 'http://www.wikidata.org/entity/Q12187714', 'http://www.wikidata.org/entity/Q12187948', 'http://www.wikidata.org/entity/Q12188030', 'http://www.wikidata.org/entity/Q12188056', 'http://www.wikidata.org/entity/Q12188617', 'http://www.wikidata.org/entity/Q12188944', 'http://www.wikidata.org/entity/Q12189023', 'http://www.wikidata.org/entity/Q12189422', 'http://www.wikidata.org/entity/Q12189449', 'http://www.wikidata.org/entity/Q12189530', 'http://www.wikidata.org/entity/Q12189776', 'http://www.wikidata.org/entity/Q12190071', 'http://www.wikidata.org/entity/Q12190227', 'http://www.wikidata.org/entity/Q12190515', 'http://www.wikidata.org/entity/Q12190542', 'http://www.wikidata.org/entity/Q12190793', 'http://www.wikidata.org/entity/Q12191144', 'http://www.wikidata.org/entity/Q12191415', 'http://www.wikidata.org/entity/Q12191447', 'http://www.wikidata.org/entity/Q12192163', 'http://www.wikidata.org/entity/Q12192260', 'http://www.wikidata.org/entity/Q12192403', 'http://www.wikidata.org/entity/Q12192449', 'http://www.wikidata.org/entity/Q12192588', 'http://www.wikidata.org/entity/Q12192860', 'http://www.wikidata.org/entity/Q12193261', 'http://www.wikidata.org/entity/Q12193560', 'http://www.wikidata.org/entity/Q12193589', 'http://www.wikidata.org/entity/Q12193707', 'http://www.wikidata.org/entity/Q12193973', 'http://www.wikidata.org/entity/Q12194422', 'http://www.wikidata.org/entity/Q12194637', 'http://www.wikidata.org/entity/Q12195127', 'http://www.wikidata.org/entity/Q12195788', 'http://www.wikidata.org/entity/Q12197874', 'http://www.wikidata.org/entity/Q12199525', 'http://www.wikidata.org/entity/Q12200476', 'http://www.wikidata.org/entity/Q12201321', 'http://www.wikidata.org/entity/Q12202359', 'http://www.wikidata.org/entity/Q122044', 'http://www.wikidata.org/entity/Q12204956', 'http://www.wikidata.org/entity/Q12207016', 'http://www.wikidata.org/entity/Q12207019', 'http://www.wikidata.org/entity/Q12207042', 'http://www.wikidata.org/entity/Q12207477', 'http://www.wikidata.org/entity/Q12209190', 'http://www.wikidata.org/entity/Q12209192', 'http://www.wikidata.org/entity/Q12209238', 'http://www.wikidata.org/entity/Q12209250', 'http://www.wikidata.org/entity/Q12209309', 'http://www.wikidata.org/entity/Q12209342', 'http://www.wikidata.org/entity/Q12209345', 'http://www.wikidata.org/entity/Q12209384', 'http://www.wikidata.org/entity/Q12209423', 'http://www.wikidata.org/entity/Q12209474', 'http://www.wikidata.org/entity/Q12209477', 'http://www.wikidata.org/entity/Q12209556', 'http://www.wikidata.org/entity/Q12209560', 'http://www.wikidata.org/entity/Q12209578', 'http://www.wikidata.org/entity/Q12209579', 'http://www.wikidata.org/entity/Q12209582', 'http://www.wikidata.org/entity/Q12209603', 'http://www.wikidata.org/entity/Q12209635', 'http://www.wikidata.org/entity/Q12209705', 'http://www.wikidata.org/entity/Q12209711', 'http://www.wikidata.org/entity/Q12209712', 'http://www.wikidata.org/entity/Q12209727', 'http://www.wikidata.org/entity/Q12209764', 'http://www.wikidata.org/entity/Q12210853', 'http://www.wikidata.org/entity/Q12211943', 'http://www.wikidata.org/entity/Q12212707', 'http://www.wikidata.org/entity/Q12213476', 'http://www.wikidata.org/entity/Q12214318', 'http://www.wikidata.org/entity/Q12215069', 'http://www.wikidata.org/entity/Q12218941', 'http://www.wikidata.org/entity/Q12219186', 'http://www.wikidata.org/entity/Q12220509', 'http://www.wikidata.org/entity/Q12220631', 'http://www.wikidata.org/entity/Q12220632', 'http://www.wikidata.org/entity/Q1222265', 'http://www.wikidata.org/entity/Q12224236', 'http://www.wikidata.org/entity/Q12227171', 'http://www.wikidata.org/entity/Q12233153', 'http://www.wikidata.org/entity/Q12233488', 'http://www.wikidata.org/entity/Q12233558', 'http://www.wikidata.org/entity/Q12234512', 'http://www.wikidata.org/entity/Q12234596', 'http://www.wikidata.org/entity/Q12234940', 'http://www.wikidata.org/entity/Q12234980', 'http://www.wikidata.org/entity/Q1223508', 'http://www.wikidata.org/entity/Q12238566', 'http://www.wikidata.org/entity/Q12238873', 'http://www.wikidata.org/entity/Q12241857', 'http://www.wikidata.org/entity/Q12241940', 'http://www.wikidata.org/entity/Q12242323', 'http://www.wikidata.org/entity/Q12242935', 'http://www.wikidata.org/entity/Q12246625', 'http://www.wikidata.org/entity/Q12248469', 'http://www.wikidata.org/entity/Q12248676', 'http://www.wikidata.org/entity/Q122758', 'http://www.wikidata.org/entity/Q122803', 'http://www.wikidata.org/entity/Q12286651', 'http://www.wikidata.org/entity/Q122881581', 'http://www.wikidata.org/entity/Q12292', 'http://www.wikidata.org/entity/Q123022482', 'http://www.wikidata.org/entity/Q123160', 'http://www.wikidata.org/entity/Q123174109', 'http://www.wikidata.org/entity/Q123196', 'http://www.wikidata.org/entity/Q123511', 'http://www.wikidata.org/entity/Q1236193', 'http://www.wikidata.org/entity/Q1236987', 'http://www.wikidata.org/entity/Q123709', 'http://www.wikidata.org/entity/Q12375138', 'http://www.wikidata.org/entity/Q1237800', 'http://www.wikidata.org/entity/Q1238323', 'http://www.wikidata.org/entity/Q1241374', 'http://www.wikidata.org/entity/Q1243772', 'http://www.wikidata.org/entity/Q1247205', 'http://www.wikidata.org/entity/Q124739', 'http://www.wikidata.org/entity/Q1249801', 'http://www.wikidata.org/entity/Q1249888', 'http://www.wikidata.org/entity/Q1249932', 'http://www.wikidata.org/entity/Q1249939', 'http://www.wikidata.org/entity/Q1250076', 'http://www.wikidata.org/entity/Q1250083', 'http://www.wikidata.org/entity/Q1250138', 'http://www.wikidata.org/entity/Q1250201', 'http://www.wikidata.org/entity/Q1250229', 'http://www.wikidata.org/entity/Q1250417', 'http://www.wikidata.org/entity/Q125080', 'http://www.wikidata.org/entity/Q1251114', 'http://www.wikidata.org/entity/Q1251242', 'http://www.wikidata.org/en</t>
+        </is>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Give me the capitals of all countries that the Himalayas run through.</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1362', 'http://www.wikidata.org/entity/Q3037', 'http://www.wikidata.org/entity/Q37400', 'http://www.wikidata.org/entity/Q5838', 'http://www.wikidata.org/entity/Q9270', 'http://www.wikidata.org/entity/Q956', 'http://www.wikidata.org/entity/Q987']</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q2807']</t>
+        </is>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>how much is the population Iraq?</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>['38274618']</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>['67326569']</t>
+        </is>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>What is the currency of the Czech Republic?</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q131016']</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q4917']</t>
+        </is>
       </c>
       <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>What is the capital of Canada?</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q1930']</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>['http://www.wikidata.org/entity/Q61']</t>
+        </is>
+      </c>
+      <c r="D6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>